<commit_message>
3 Sum solved + Notes
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143D3E2E-FB43-4AA2-BE36-3B22AED644D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007179E6-A33E-4D5B-B912-B07A0C93717E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -152,6 +152,15 @@
   </si>
   <si>
     <t>isStrictlyPalindromic</t>
+  </si>
+  <si>
+    <t>Sort first, iterate trough all with one pointer to the second number and a the other to the last. Increment or decrement these indexes as required To mind the edge cases with 3+ equual numbers, (de)increment while the following number is the same</t>
+  </si>
+  <si>
+    <t>ThreeSum</t>
+  </si>
+  <si>
+    <t>TwoSum II</t>
   </si>
 </sst>
 </file>
@@ -205,11 +214,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,7 +575,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,11 +857,35 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1882,7 +1918,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1213">
+  <conditionalFormatting sqref="C1:C13 C15:C1213">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",C1)))</formula>
     </cfRule>
@@ -1907,7 +1943,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C1:C1213</xm:sqref>
+          <xm:sqref>C1:C13 C15:C1213</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Challenge number #150 complete
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007179E6-A33E-4D5B-B912-B07A0C93717E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A8FD17-9554-475D-891D-F6E4B7A03454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>TwoSum II</t>
+  </si>
+  <si>
+    <t>Convert string to int with stoi(), then push it to stack if its a number, else (aka operand) make two pops and do the respective calc. Key part is pushing the solution back to the stack, so it is first parameter of the next calculation</t>
+  </si>
+  <si>
+    <t>evalRPN</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,6 +896,21 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
This challenge is too hard for my current level, decided to go for something else
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A8FD17-9554-475D-891D-F6E4B7A03454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D14C50-243F-43FD-800C-A1444E225503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -167,13 +167,19 @@
   </si>
   <si>
     <t>evalRPN</t>
+  </si>
+  <si>
+    <t>347. Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t>learnt pretty much nothing, this is too hard of a challenge, decided to practice more easy array examples, and didn’t count it as an example</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,8 +193,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +228,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -216,11 +242,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -228,8 +270,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -581,7 +628,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -913,82 +960,97 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Did another exercise today
We have two #17 because previous count was wrong

Loop where u add the next value to the overall saved sum
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E52EB3-8A09-44FE-8721-0109CEAAC47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DDE9B0-DDAA-44A0-8F5C-7DE39EFDE916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>Generate Valid parenthesis</t>
+  </si>
+  <si>
+    <t>Loop where u add the next value to the overall saved sum</t>
+  </si>
+  <si>
+    <t>runningSum</t>
   </si>
 </sst>
 </file>
@@ -657,7 +663,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,6 +1078,21 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
+      </c>
+      <c r="B21">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Incomplete 019 - Redo
easy one, but had mw day before and was too tired for this and dind't want to peak the solution as it seemed rather easy.

Unordered map doesnt even make sense, that s when is stoped
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD30EF4-F0CA-4A6C-AA4A-444852601BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27234B76-0606-4C81-B1DE-AA25FBEF7128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -203,6 +203,18 @@
   </si>
   <si>
     <t>Calculate prefix products forward, then postfix backwards in a 2nd pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typical exercise for sliding window algorithm, increases the window while letter is different, reset once it is the same </t>
+  </si>
+  <si>
+    <t>13 missed 1</t>
+  </si>
+  <si>
+    <t>REDO</t>
+  </si>
+  <si>
+    <t>lengthOfLongestSubstring</t>
   </si>
 </sst>
 </file>
@@ -324,14 +336,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -669,13 +681,13 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
@@ -1125,6 +1137,21 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2118,7 +2145,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C13 C15:C1213">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Commit of #21 solution
Introduction to binary search
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E13A64-1CDF-42FF-8A54-53029D0AB457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288FEBA7-3AB0-4B24-9A03-71A2796EB6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -215,13 +215,25 @@
   </si>
   <si>
     <t>lengthOfLongestSubstring</t>
+  </si>
+  <si>
+    <t>Since  the array is sorted this is a clear angle for  Binary Search</t>
+  </si>
+  <si>
+    <t>missed 1</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +264,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A9955"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -309,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -325,6 +343,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -681,7 +702,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B17" sqref="A17:XFD17"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,10 +1198,29 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
+      </c>
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
024 Random exercise i did
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABFAE5C-97CD-45F2-90D3-16743B6BE94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C89581F-40FC-4958-AF55-16F394BB9E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>invertTree</t>
+  </si>
+  <si>
+    <t>numIdenticalPairs</t>
+  </si>
+  <si>
+    <t>Great exercise to understand how you can populate an unordered map and do the math at the same time. Great exercise to achieve O(n)</t>
   </si>
 </sst>
 </file>
@@ -717,7 +723,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,6 +1287,21 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
+      </c>
+      <c r="B29">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
029 - Binary Search DFS
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C89581F-40FC-4958-AF55-16F394BB9E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C32391-EE91-4708-A4B6-CB33B7E511DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>Great exercise to understand how you can populate an unordered map and do the math at the same time. Great exercise to achieve O(n)</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>Did by myself which means I understood the previous teachings on DFS. It is a simple aplication of that</t>
   </si>
 </sst>
 </file>
@@ -723,7 +729,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,93 +1314,126 @@
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
[Arrays] Roman To Integer
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FD274E-CB53-41EF-898A-9A7CA8F67695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84AFBFA-7C8F-4E4B-93D4-6A5115FF4308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -260,6 +260,21 @@
   </si>
   <si>
     <t>This one has a weird solution, that is hard to find out, but easy to code out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy,made by myself. Had to peak the solutions to correct some of my mistakes but it was fine. Belongs to the 100 most liked questions on Leetcode </t>
+  </si>
+  <si>
+    <t>searchInsert</t>
+  </si>
+  <si>
+    <t>Top Liked</t>
+  </si>
+  <si>
+    <t>romanToInt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy. Just add the following number, but be careful with the final edge case. Had to peak the solutions tho. Belongs to the 100 most liked questions on Leetcode </t>
   </si>
 </sst>
 </file>
@@ -307,7 +322,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +344,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -360,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -381,6 +402,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -734,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CE9E97-2B99-405F-AEFD-436D25B2305A}">
   <dimension ref="A1:L221"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +770,7 @@
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="135.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="135.7109375" customWidth="1"/>
     <col min="7" max="9" width="11" customWidth="1"/>
     <col min="10" max="12" width="12" customWidth="1"/>
   </cols>
@@ -1387,6 +1412,18 @@
       <c r="B35">
         <v>25</v>
       </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -1394,6 +1431,18 @@
       </c>
       <c r="B36">
         <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pascals Tringle - Should redo with recursion
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84AFBFA-7C8F-4E4B-93D4-6A5115FF4308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE933CDC-F2E4-41AE-BCD8-81D3D70A18DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t xml:space="preserve">Easy. Just add the following number, but be careful with the final edge case. Had to peak the solutions tho. Belongs to the 100 most liked questions on Leetcode </t>
+  </si>
+  <si>
+    <t>Easy. Had some problems since i was accessing outside of memory. There is a way to solve this using recursion which i should try next</t>
+  </si>
+  <si>
+    <t>Pascal's Triangle</t>
   </si>
 </sst>
 </file>
@@ -381,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -406,6 +412,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -461,9 +470,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -501,7 +510,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -607,7 +616,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -749,7 +758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CE9E97-2B99-405F-AEFD-436D25B2305A}">
   <dimension ref="A1:L221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,6 +1457,21 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
+      </c>
+      <c r="B37">
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Recursion solution for Pascal's Triangle
Wanted to check out the recursion solutionfor this problem. Added some pritnfs to better understand
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE933CDC-F2E4-41AE-BCD8-81D3D70A18DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1245997C-7CA1-4CF6-8E31-7BE325E6C29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t>Pascal's Triangle</t>
+  </si>
+  <si>
+    <t>Wanted to check out the recursion solutionfor this problem. Added some pritnfs to better understand</t>
   </si>
 </sst>
 </file>
@@ -769,7 +772,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,6 +1480,21 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
+      </c>
+      <c r="B38">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sort Colors: Dutch National Flag Algorithm (aka 3 pointers)
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1245997C-7CA1-4CF6-8E31-7BE325E6C29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F84A21-D857-4843-898A-B1113AA8AA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="85">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>Wanted to check out the recursion solutionfor this problem. Added some pritnfs to better understand</t>
+  </si>
+  <si>
+    <t>From the description of the Dutch Flag algorithm ended up finding the solution. Just with the 2 pointers Algorithm, finding a solution was not possible I believe</t>
+  </si>
+  <si>
+    <t>Sort Colors</t>
   </si>
 </sst>
 </file>
@@ -772,7 +778,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,6 +1506,21 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
+      </c>
+      <c r="B39">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#2610. Convert an Array Into a 2D Array With Conditions
Great Exercise, solved with ease
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amaral\GitRepos\LeetCode-Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F84A21-D857-4843-898A-B1113AA8AA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2C8674-4777-416D-8D81-A74774568BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0726A895-2255-4A1C-8358-142053C22366}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
   <si>
     <t>containsDuplicate</t>
   </si>
@@ -290,6 +290,24 @@
   </si>
   <si>
     <t>Sort Colors</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>findMatrix</t>
+  </si>
+  <si>
+    <t>Good medium challenge, took me 40min but managed to reach the right "algorithm" by myself - with great runtime too -</t>
+  </si>
+  <si>
+    <t>42 School</t>
+  </si>
+  <si>
+    <t>ft_print_comb</t>
+  </si>
+  <si>
+    <t>create a function that displays all different combinations of three different digits in ascending order, listed by ascending order - yes, repetition is voluntary.</t>
   </si>
 </sst>
 </file>
@@ -479,9 +497,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -519,7 +537,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -625,7 +643,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -767,7 +785,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -778,7 +796,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="G32" sqref="G31:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,10 +1545,37 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
+      </c>
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>